<commit_message>
Redmine ticket 8570 cal sheets for GP05MOAS-GL001 and GP05MOAS-GL002 modified.
</commit_message>
<xml_diff>
--- a/GP05MOAS-GL001/Omaha_Cal_Info_GP05MOAS-GL001_00001.xlsx
+++ b/GP05MOAS-GL001/Omaha_Cal_Info_GP05MOAS-GL001_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Sheets from -test 2015-08-19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Repaired GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="12720" windowHeight="12408" tabRatio="377" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18264" windowHeight="8052" tabRatio="377" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -406,7 +406,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,6 +434,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,7 +524,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -592,6 +598,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1088,7 +1097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -1218,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1291,8 +1300,8 @@
       <c r="E4" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="30">
-        <v>117</v>
+      <c r="F4" s="31">
+        <v>140</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>52</v>
@@ -1339,8 +1348,8 @@
       <c r="E6" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="30">
-        <v>1.08</v>
+      <c r="F6" s="31">
+        <v>1.1299999999999999</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>52</v>

</xml_diff>